<commit_message>
Updates to source files
</commit_message>
<xml_diff>
--- a/SupportingDocs/Calculators/WDT_Areej.xlsx
+++ b/SupportingDocs/Calculators/WDT_Areej.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\Coding\Masters\SupportingDocs\Calculators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D025995-2D4E-4485-98C3-61937A1A9F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DD3A7F-DAEF-4CB8-BD08-C8DA3B4F5121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6FE154D1-9408-484E-8BBE-1ECE0188AFD8}"/>
   </bookViews>
@@ -159,9 +159,6 @@
     <t>24s8pole</t>
   </si>
   <si>
-    <t>24s4pole</t>
-  </si>
-  <si>
     <t>shift</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>yc</t>
+  </si>
+  <si>
+    <t>24s2p</t>
   </si>
 </sst>
 </file>
@@ -355,22 +355,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -378,50 +373,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1295257-16CD-4001-9DF2-C6F519FD2D00}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -766,7 +754,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -799,7 +787,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -834,7 +822,7 @@
       </c>
       <c r="C8">
         <f>C6*(C2-C3)/(2*C4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -846,7 +834,7 @@
       </c>
       <c r="C9">
         <f>C6*C2/(2*C4*C10)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -858,7 +846,7 @@
       </c>
       <c r="C10">
         <f>GCD(C2,C5)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -882,7 +870,7 @@
       </c>
       <c r="C12">
         <f>(C2-C3)/(2*C5*C4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -906,7 +894,7 @@
       </c>
       <c r="C14">
         <f>C2/(C6*C5*C4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -915,7 +903,7 @@
       </c>
       <c r="C15">
         <f>FLOOR(C12,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -933,7 +921,7 @@
       </c>
       <c r="C17">
         <f>GCD(C16,C5)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -942,7 +930,7 @@
       </c>
       <c r="C18">
         <f>C2/C17</f>
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -963,7 +951,7 @@
       </c>
       <c r="C20">
         <f>2*C4*C8/C4</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -980,10 +968,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="C22">
         <f>(C4-1)/2</f>
@@ -991,21 +979,21 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="13" t="s">
-        <v>51</v>
+      <c r="B23" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="C23">
         <f>C2/(2*C5)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="13" t="s">
-        <v>52</v>
+      <c r="B24" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="C24">
         <f>C23*5/6</f>
-        <v>2.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1018,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867518C4-0CB7-4184-8BB9-867B8EA9A39B}">
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N42" sqref="N41:N42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1032,80 +1020,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="36"/>
+      <c r="D1" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="25" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27">
-        <v>2</v>
-      </c>
-      <c r="D3" s="27">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20">
+        <v>2</v>
+      </c>
+      <c r="D3" s="20">
         <v>3</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="20">
         <v>4</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="20">
         <v>5</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="20">
         <v>6</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="20">
         <v>7</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+      <c r="A4" s="19">
         <v>1</v>
       </c>
       <c r="B4" s="3">
@@ -1117,24 +1105,24 @@
       <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="3">
         <v>14</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="4">
         <v>3</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="5">
         <v>15</v>
       </c>
       <c r="H4" s="5">
         <v>4</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="11">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="26">
+      <c r="A5" s="19">
         <v>2</v>
       </c>
       <c r="B5" s="7">
@@ -1146,126 +1134,126 @@
       <c r="D5" s="7">
         <v>6</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="7">
         <v>18</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="2">
         <v>7</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="3">
         <v>19</v>
       </c>
       <c r="H5" s="3">
         <v>8</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="9">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="37">
+      <c r="A6" s="23">
         <v>3</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="24">
         <v>9</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="24">
         <v>21</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="24">
         <v>10</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="24">
         <v>22</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="25">
         <v>11</v>
       </c>
-      <c r="G6" s="41">
+      <c r="G6" s="26">
         <v>23</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="26">
         <v>12</v>
       </c>
-      <c r="I6" s="43">
+      <c r="I6" s="27">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="36"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="25" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27">
-        <v>1</v>
-      </c>
-      <c r="C10" s="27">
-        <v>2</v>
-      </c>
-      <c r="D10" s="27">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20">
+        <v>1</v>
+      </c>
+      <c r="C10" s="20">
+        <v>2</v>
+      </c>
+      <c r="D10" s="20">
         <v>3</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="20">
         <v>4</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="20">
         <v>5</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="20">
         <v>6</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="20">
         <v>7</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="21">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="26">
+      <c r="A11" s="19">
         <v>1</v>
       </c>
       <c r="B11" s="3">
@@ -1277,24 +1265,24 @@
       <c r="D11" s="3">
         <v>13</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="3">
         <v>19</v>
       </c>
-      <c r="F11" s="11">
-        <v>2</v>
-      </c>
-      <c r="G11" s="12">
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="5">
         <v>8</v>
       </c>
       <c r="H11" s="5">
         <v>14</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="11">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="26">
+      <c r="A12" s="19">
         <v>2</v>
       </c>
       <c r="B12" s="7">
@@ -1306,160 +1294,152 @@
       <c r="D12" s="7">
         <v>15</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <v>21</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="2">
         <v>4</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="3">
         <v>10</v>
       </c>
       <c r="H12" s="3">
         <v>16</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="9">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="37">
+      <c r="A13" s="23">
         <v>3</v>
       </c>
-      <c r="B13" s="38">
+      <c r="B13" s="24">
         <v>5</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="24">
         <v>11</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="24">
         <v>17</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E13" s="24">
         <v>23</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="25">
         <v>6</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="26">
         <v>12</v>
       </c>
-      <c r="H13" s="42">
+      <c r="H13" s="26">
         <v>18</v>
       </c>
-      <c r="I13" s="43">
+      <c r="I13" s="27">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="22"/>
+      <c r="D15" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="16"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="25"/>
+      <c r="A16" s="17"/>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="S16" s="18"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27">
-        <v>1</v>
-      </c>
-      <c r="C17" s="27">
-        <v>2</v>
-      </c>
-      <c r="D17" s="27">
+      <c r="A17" s="19"/>
+      <c r="B17" s="20">
+        <v>1</v>
+      </c>
+      <c r="C17" s="20">
+        <v>2</v>
+      </c>
+      <c r="D17" s="20">
         <v>3</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="20">
         <v>4</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="20">
         <v>5</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="20">
         <v>6</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H17" s="20">
         <v>7</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I17" s="20">
         <v>8</v>
       </c>
-      <c r="J17" s="27">
+      <c r="J17" s="20">
         <v>9</v>
       </c>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="28"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="21"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="26">
+      <c r="A18" s="19">
         <v>1</v>
       </c>
       <c r="B18" s="3">
@@ -1471,13 +1451,13 @@
       <c r="D18" s="3">
         <v>10</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="3">
         <v>11</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="3">
         <v>19</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="3">
         <v>20</v>
       </c>
       <c r="H18" s="4">
@@ -1486,21 +1466,13 @@
       <c r="I18" s="5">
         <v>-12</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="5">
         <v>-21</v>
       </c>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="25"/>
+      <c r="S18" s="18"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="26">
+      <c r="A19" s="19">
         <v>2</v>
       </c>
       <c r="B19" s="7">
@@ -1512,13 +1484,13 @@
       <c r="D19" s="7">
         <v>13</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="7">
         <v>14</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="7">
         <v>22</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="7">
         <v>23</v>
       </c>
       <c r="H19" s="2">
@@ -1527,21 +1499,13 @@
       <c r="I19" s="3">
         <v>-15</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="3">
         <v>-24</v>
       </c>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="25"/>
+      <c r="S19" s="18"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="26">
+      <c r="A20" s="19">
         <v>3</v>
       </c>
       <c r="B20" s="5">
@@ -1550,16 +1514,16 @@
       <c r="C20" s="5">
         <v>8</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="5">
         <v>16</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="5">
         <v>17</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="5">
         <v>25</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="5">
         <v>26</v>
       </c>
       <c r="H20" s="6">
@@ -1568,39 +1532,14 @@
       <c r="I20" s="7">
         <v>-18</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="7">
         <v>-27</v>
       </c>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="25"/>
+      <c r="S20" s="18"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="25"/>
+      <c r="A21" s="17"/>
+      <c r="S21" s="18"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
@@ -1612,141 +1551,132 @@
       <c r="C22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="25"/>
+      <c r="D22" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="K23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="L23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="M23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N23" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="O23" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="P23" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q23" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="R23" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="S23" s="25" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" t="s">
+        <v>36</v>
+      </c>
+      <c r="M23" t="s">
+        <v>36</v>
+      </c>
+      <c r="N23" t="s">
+        <v>20</v>
+      </c>
+      <c r="O23" t="s">
+        <v>20</v>
+      </c>
+      <c r="P23" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>20</v>
+      </c>
+      <c r="R23" t="s">
+        <v>20</v>
+      </c>
+      <c r="S23" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27">
-        <v>1</v>
-      </c>
-      <c r="C24" s="27">
-        <v>2</v>
-      </c>
-      <c r="D24" s="27">
+      <c r="A24" s="19"/>
+      <c r="B24" s="20">
+        <v>1</v>
+      </c>
+      <c r="C24" s="20">
+        <v>2</v>
+      </c>
+      <c r="D24" s="20">
         <v>3</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="20">
         <v>4</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="20">
         <v>5</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="20">
         <v>6</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24" s="20">
         <v>7</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I24" s="20">
         <v>8</v>
       </c>
-      <c r="J24" s="27">
+      <c r="J24" s="20">
         <v>9</v>
       </c>
-      <c r="K24" s="27">
+      <c r="K24" s="20">
         <v>10</v>
       </c>
-      <c r="L24" s="27">
+      <c r="L24" s="20">
         <v>11</v>
       </c>
-      <c r="M24" s="27">
+      <c r="M24" s="20">
         <v>12</v>
       </c>
-      <c r="N24" s="27">
+      <c r="N24" s="20">
         <v>13</v>
       </c>
-      <c r="O24" s="27">
+      <c r="O24" s="20">
         <v>14</v>
       </c>
-      <c r="P24" s="27">
+      <c r="P24" s="20">
         <v>15</v>
       </c>
-      <c r="Q24" s="27">
+      <c r="Q24" s="20">
         <v>16</v>
       </c>
-      <c r="R24" s="27">
+      <c r="R24" s="20">
         <v>17</v>
       </c>
-      <c r="S24" s="28">
+      <c r="S24" s="21">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25" s="26">
+      <c r="A25" s="19">
         <v>1</v>
       </c>
       <c r="B25" s="3">
@@ -1764,48 +1694,48 @@
       <c r="F25" s="3">
         <v>10</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="3">
         <v>-14</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="3">
         <v>11</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="3">
         <v>-15</v>
       </c>
-      <c r="J25" s="8">
+      <c r="J25" s="3">
         <v>19</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="3">
         <v>-23</v>
       </c>
-      <c r="L25" s="8">
-        <v>20</v>
-      </c>
-      <c r="M25" s="8">
+      <c r="L25" s="3">
+        <v>20</v>
+      </c>
+      <c r="M25" s="3">
         <v>-24</v>
       </c>
       <c r="N25" s="2">
         <v>-6</v>
       </c>
-      <c r="O25" s="8">
+      <c r="O25" s="3">
         <v>10</v>
       </c>
       <c r="P25" s="3">
         <v>-15</v>
       </c>
-      <c r="Q25" s="8">
+      <c r="Q25" s="3">
         <v>19</v>
       </c>
-      <c r="R25" s="8">
+      <c r="R25" s="3">
         <v>-24</v>
       </c>
-      <c r="S25" s="30">
+      <c r="S25" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26" s="26">
+      <c r="A26" s="19">
         <v>2</v>
       </c>
       <c r="B26" s="7">
@@ -1826,19 +1756,19 @@
       <c r="G26" s="7">
         <v>-17</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="7">
         <v>14</v>
       </c>
       <c r="I26" s="7">
         <v>-18</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="7">
         <v>22</v>
       </c>
       <c r="K26" s="7">
         <v>-26</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="7">
         <v>23</v>
       </c>
       <c r="M26" s="7">
@@ -1847,24 +1777,24 @@
       <c r="N26" s="6">
         <v>-9</v>
       </c>
-      <c r="O26" s="10">
+      <c r="O26" s="7">
         <v>13</v>
       </c>
       <c r="P26" s="7">
         <v>-18</v>
       </c>
-      <c r="Q26" s="10">
+      <c r="Q26" s="7">
         <v>22</v>
       </c>
-      <c r="R26" s="10">
+      <c r="R26" s="7">
         <v>-27</v>
       </c>
-      <c r="S26" s="31">
+      <c r="S26" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="26">
+      <c r="A27" s="19">
         <v>3</v>
       </c>
       <c r="B27" s="5">
@@ -1879,25 +1809,25 @@
       <c r="E27" s="5">
         <v>-12</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="5">
         <v>16</v>
       </c>
       <c r="G27" s="5">
         <v>-20</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="5">
         <v>17</v>
       </c>
       <c r="I27" s="5">
         <v>-21</v>
       </c>
-      <c r="J27" s="12">
+      <c r="J27" s="5">
         <v>25</v>
       </c>
       <c r="K27" s="5">
         <v>-2</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="5">
         <v>26</v>
       </c>
       <c r="M27" s="5">
@@ -1906,112 +1836,106 @@
       <c r="N27" s="4">
         <v>-3</v>
       </c>
-      <c r="O27" s="12">
+      <c r="O27" s="5">
         <v>7</v>
       </c>
       <c r="P27" s="5">
         <v>-12</v>
       </c>
-      <c r="Q27" s="12">
+      <c r="Q27" s="5">
         <v>16</v>
       </c>
-      <c r="R27" s="12">
+      <c r="R27" s="5">
         <v>-21</v>
       </c>
-      <c r="S27" s="32">
+      <c r="S27" s="11">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="33"/>
-      <c r="B28" s="34" t="s">
+      <c r="A28" s="22"/>
+      <c r="B28" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34" t="s">
+      <c r="O28" s="35"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="36"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="O28" s="34"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
-      <c r="S28" s="35"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="36"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="38"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="25"/>
+      <c r="A31" s="17"/>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A32" s="23"/>
-      <c r="B32" s="44">
-        <v>1</v>
-      </c>
-      <c r="C32" s="44">
-        <v>2</v>
-      </c>
-      <c r="D32" s="44">
+      <c r="A32" s="17"/>
+      <c r="B32" s="28">
+        <v>1</v>
+      </c>
+      <c r="C32" s="28">
+        <v>2</v>
+      </c>
+      <c r="D32" s="28">
         <v>3</v>
       </c>
-      <c r="E32" s="44">
+      <c r="E32" s="28">
         <v>4</v>
       </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="25"/>
+      <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A33" s="45">
+      <c r="A33" s="29">
         <v>1</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="9">
         <v>2</v>
       </c>
       <c r="D33" s="5">
@@ -2020,19 +1944,16 @@
       <c r="E33" s="5">
         <v>4</v>
       </c>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="25"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A34" s="45">
+      <c r="A34" s="29">
         <v>2</v>
       </c>
       <c r="B34" s="7">
         <v>5</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="10">
         <v>6</v>
       </c>
       <c r="D34" s="3">
@@ -2041,212 +1962,193 @@
       <c r="E34" s="3">
         <v>8</v>
       </c>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="25"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A35" s="46">
+      <c r="A35" s="30">
         <v>3</v>
       </c>
-      <c r="B35" s="38">
+      <c r="B35" s="24">
         <v>9</v>
       </c>
-      <c r="C35" s="47">
+      <c r="C35" s="31">
         <v>10</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="26">
         <v>11</v>
       </c>
-      <c r="E35" s="42">
+      <c r="E35" s="26">
         <v>12</v>
       </c>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="49"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="33"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="36"/>
+      <c r="D37" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="38"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="25"/>
+      <c r="A38" s="17"/>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="18"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A39" s="23"/>
-      <c r="B39" s="44">
-        <v>1</v>
-      </c>
-      <c r="C39" s="44">
-        <v>2</v>
-      </c>
-      <c r="D39" s="44">
+      <c r="A39" s="17"/>
+      <c r="B39" s="28">
+        <v>1</v>
+      </c>
+      <c r="C39" s="28">
+        <v>2</v>
+      </c>
+      <c r="D39" s="28">
         <v>3</v>
       </c>
-      <c r="E39" s="44"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="25"/>
+      <c r="E39" s="28"/>
+      <c r="I39" s="18"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A40" s="45">
+      <c r="A40" s="29">
         <v>1</v>
       </c>
       <c r="B40" s="3">
         <v>1</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="9">
         <v>8</v>
       </c>
       <c r="D40" s="5">
         <v>6</v>
       </c>
       <c r="E40" s="5"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="25"/>
+      <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A41" s="45">
+      <c r="A41" s="29">
         <v>2</v>
       </c>
       <c r="B41" s="7">
         <v>4</v>
       </c>
-      <c r="C41" s="15">
+      <c r="C41" s="10">
         <v>2</v>
       </c>
       <c r="D41" s="3">
         <v>4</v>
       </c>
       <c r="E41" s="3"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="25"/>
+      <c r="I41" s="18"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A42" s="46">
+      <c r="A42" s="30">
         <v>3</v>
       </c>
-      <c r="B42" s="38">
+      <c r="B42" s="24">
         <v>7</v>
       </c>
-      <c r="C42" s="47">
+      <c r="C42" s="31">
         <v>5</v>
       </c>
-      <c r="D42" s="42">
+      <c r="D42" s="26">
         <v>3</v>
       </c>
-      <c r="E42" s="42"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="49"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="33"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="21"/>
-      <c r="L44" s="21"/>
-      <c r="M44" s="21"/>
-      <c r="N44" s="21"/>
-      <c r="O44" s="21"/>
-      <c r="P44" s="22"/>
+      <c r="D44" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="16"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A45" s="26"/>
-      <c r="B45" s="27">
-        <v>1</v>
-      </c>
-      <c r="C45" s="27">
-        <v>2</v>
-      </c>
-      <c r="D45" s="24"/>
-      <c r="E45" s="27">
+      <c r="A45" s="19"/>
+      <c r="B45" s="20">
+        <v>1</v>
+      </c>
+      <c r="C45" s="20">
+        <v>2</v>
+      </c>
+      <c r="E45" s="20">
         <v>3</v>
       </c>
-      <c r="F45" s="27">
+      <c r="F45" s="20">
         <v>4</v>
       </c>
-      <c r="G45" s="24"/>
-      <c r="H45" s="27">
+      <c r="H45" s="20">
         <v>5</v>
       </c>
-      <c r="I45" s="27">
+      <c r="I45" s="20">
         <v>6</v>
       </c>
-      <c r="J45" s="24"/>
-      <c r="K45" s="27">
-        <v>1</v>
-      </c>
-      <c r="L45" s="27">
-        <v>2</v>
-      </c>
-      <c r="M45" s="27">
+      <c r="K45" s="20">
+        <v>1</v>
+      </c>
+      <c r="L45" s="20">
+        <v>2</v>
+      </c>
+      <c r="M45" s="20">
         <v>3</v>
       </c>
-      <c r="N45" s="27">
+      <c r="N45" s="20">
         <v>4</v>
       </c>
-      <c r="O45" s="27">
+      <c r="O45" s="20">
         <v>5</v>
       </c>
-      <c r="P45" s="28">
+      <c r="P45" s="21">
         <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A46" s="26">
+      <c r="A46" s="19">
         <v>1</v>
       </c>
       <c r="B46" s="3">
@@ -2255,21 +2157,18 @@
       <c r="C46" s="4">
         <v>2</v>
       </c>
-      <c r="D46" s="24"/>
       <c r="E46" s="3">
         <v>7</v>
       </c>
       <c r="F46" s="4">
         <v>8</v>
       </c>
-      <c r="G46" s="24"/>
       <c r="H46" s="3">
         <v>13</v>
       </c>
-      <c r="I46" s="11">
+      <c r="I46" s="4">
         <v>14</v>
       </c>
-      <c r="J46" s="24"/>
       <c r="K46" s="3">
         <v>1</v>
       </c>
@@ -2285,12 +2184,12 @@
       <c r="O46" s="5">
         <v>8</v>
       </c>
-      <c r="P46" s="32">
+      <c r="P46" s="11">
         <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A47" s="26">
+      <c r="A47" s="19">
         <v>2</v>
       </c>
       <c r="B47" s="7">
@@ -2299,7 +2198,7 @@
       <c r="C47" s="2">
         <v>4</v>
       </c>
-      <c r="D47" s="50" t="s">
+      <c r="D47" s="34" t="s">
         <v>36</v>
       </c>
       <c r="E47" s="7">
@@ -2308,7 +2207,7 @@
       <c r="F47" s="2">
         <v>10</v>
       </c>
-      <c r="G47" s="50" t="s">
+      <c r="G47" s="34" t="s">
         <v>36</v>
       </c>
       <c r="H47" s="7">
@@ -2317,8 +2216,8 @@
       <c r="I47" s="2">
         <v>16</v>
       </c>
-      <c r="J47" s="50" t="s">
-        <v>50</v>
+      <c r="J47" s="34" t="s">
+        <v>49</v>
       </c>
       <c r="K47" s="7">
         <v>3</v>
@@ -2335,51 +2234,51 @@
       <c r="O47" s="3">
         <v>10</v>
       </c>
-      <c r="P47" s="14">
+      <c r="P47" s="9">
         <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A48" s="37">
+      <c r="A48" s="23">
         <v>3</v>
       </c>
-      <c r="B48" s="38">
+      <c r="B48" s="24">
         <v>5</v>
       </c>
-      <c r="C48" s="51">
+      <c r="C48" s="25">
         <v>6</v>
       </c>
-      <c r="D48" s="48"/>
-      <c r="E48" s="38">
+      <c r="D48" s="32"/>
+      <c r="E48" s="24">
         <v>11</v>
       </c>
-      <c r="F48" s="51">
+      <c r="F48" s="25">
         <v>12</v>
       </c>
-      <c r="G48" s="48"/>
-      <c r="H48" s="39">
+      <c r="G48" s="32"/>
+      <c r="H48" s="24">
         <v>17</v>
       </c>
-      <c r="I48" s="51">
+      <c r="I48" s="25">
         <v>18</v>
       </c>
-      <c r="J48" s="48"/>
-      <c r="K48" s="38">
+      <c r="J48" s="32"/>
+      <c r="K48" s="24">
         <v>5</v>
       </c>
-      <c r="L48" s="38">
+      <c r="L48" s="24">
         <v>11</v>
       </c>
-      <c r="M48" s="39">
+      <c r="M48" s="24">
         <v>17</v>
       </c>
-      <c r="N48" s="51">
+      <c r="N48" s="25">
         <v>6</v>
       </c>
-      <c r="O48" s="42">
+      <c r="O48" s="26">
         <v>12</v>
       </c>
-      <c r="P48" s="43">
+      <c r="P48" s="27">
         <v>18</v>
       </c>
     </row>

</xml_diff>